<commit_message>
Updated for day 8
</commit_message>
<xml_diff>
--- a/ExcelEsport/Dim bootcamp notes.xlsx
+++ b/ExcelEsport/Dim bootcamp notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\ExcelEsport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2948472F-0103-42F6-BE6F-669AD684E0E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CB7B3E-89BA-4E4D-9C62-2D64D07C1897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="5" xr2:uid="{F9BF1E89-DD97-4488-B5FA-5A3F8B8826CF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="9" xr2:uid="{F9BF1E89-DD97-4488-B5FA-5A3F8B8826CF}"/>
   </bookViews>
   <sheets>
     <sheet name="D1" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <definedName name="names">'D1 ex'!$B$13</definedName>
     <definedName name="Team_2D">'D8 ex'!$A$3:$A$6</definedName>
   </definedNames>
-  <calcPr calcId="191028" calcOnSave="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2525,10 +2525,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B07696C6-41DC-4867-AC84-E6097DFBBB4D}">
   <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C56" sqref="C56"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="47.4" x14ac:dyDescent="0.9"/>
@@ -3014,8 +3014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2EE8F1C-EAAA-4794-892B-BC309416F003}">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showGridLines="0" topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.9375" defaultRowHeight="27.45" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -3027,7 +3027,7 @@
     <col min="5" max="5" width="5.9375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.87890625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.76171875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.87890625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.64453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.41015625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.46875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.234375" bestFit="1" customWidth="1"/>
@@ -3271,6 +3271,10 @@
         <f t="array" ref="C10:C57">_xlfn.TOCOL(Data_2D)</f>
         <v>0</v>
       </c>
+      <c r="E10" t="str" cm="1">
+        <f t="array" ref="E10:E57">_xlfn.TOCOL(IF(Data_2D&lt;&gt;-1,Month_2D))</f>
+        <v>Jan</v>
+      </c>
     </row>
     <row r="11" spans="1:13" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" t="str">
@@ -3282,6 +3286,9 @@
       <c r="C11">
         <v>12</v>
       </c>
+      <c r="E11" t="str">
+        <v>Feb</v>
+      </c>
     </row>
     <row r="12" spans="1:13" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" t="str">
@@ -3293,6 +3300,9 @@
       <c r="C12">
         <v>35</v>
       </c>
+      <c r="E12" t="str">
+        <v>Mar</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" t="str">
@@ -3304,6 +3314,9 @@
       <c r="C13">
         <v>38</v>
       </c>
+      <c r="E13" t="str">
+        <v>Apr</v>
+      </c>
     </row>
     <row r="14" spans="1:13" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" t="str">
@@ -3315,6 +3328,9 @@
       <c r="C14">
         <v>28</v>
       </c>
+      <c r="E14" t="str">
+        <v>May</v>
+      </c>
     </row>
     <row r="15" spans="1:13" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A15" t="str">
@@ -3326,6 +3342,9 @@
       <c r="C15">
         <v>31</v>
       </c>
+      <c r="E15" t="str">
+        <v>Jun</v>
+      </c>
     </row>
     <row r="16" spans="1:13" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" t="str">
@@ -3337,8 +3356,11 @@
       <c r="C16">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E16" t="str">
+        <v>Jul</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A17" t="str">
         <v>Team Alpha</v>
       </c>
@@ -3348,8 +3370,11 @@
       <c r="C17">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E17" t="str">
+        <v>Aug</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A18" t="str">
         <v>Team Alpha</v>
       </c>
@@ -3359,8 +3384,11 @@
       <c r="C18">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E18" t="str">
+        <v>Sep</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A19" t="str">
         <v>Team Alpha</v>
       </c>
@@ -3370,8 +3398,11 @@
       <c r="C19">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E19" t="str">
+        <v>Oct</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A20" t="str">
         <v>Team Alpha</v>
       </c>
@@ -3381,8 +3412,11 @@
       <c r="C20">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E20" t="str">
+        <v>Nov</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A21" t="str">
         <v>Team Alpha</v>
       </c>
@@ -3392,8 +3426,11 @@
       <c r="C21">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E21" t="str">
+        <v>Dec</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A22" t="str">
         <v>Team Beta</v>
       </c>
@@ -3403,8 +3440,11 @@
       <c r="C22">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E22" t="str">
+        <v>Jan</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A23" t="str">
         <v>Team Beta</v>
       </c>
@@ -3414,8 +3454,11 @@
       <c r="C23">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E23" t="str">
+        <v>Feb</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A24" t="str">
         <v>Team Beta</v>
       </c>
@@ -3425,8 +3468,11 @@
       <c r="C24">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E24" t="str">
+        <v>Mar</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A25" t="str">
         <v>Team Beta</v>
       </c>
@@ -3436,8 +3482,11 @@
       <c r="C25">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E25" t="str">
+        <v>Apr</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A26" t="str">
         <v>Team Beta</v>
       </c>
@@ -3447,8 +3496,11 @@
       <c r="C26">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E26" t="str">
+        <v>May</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A27" t="str">
         <v>Team Beta</v>
       </c>
@@ -3458,8 +3510,11 @@
       <c r="C27">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E27" t="str">
+        <v>Jun</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A28" t="str">
         <v>Team Beta</v>
       </c>
@@ -3469,8 +3524,11 @@
       <c r="C28">
         <v>34</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E28" t="str">
+        <v>Jul</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A29" t="str">
         <v>Team Beta</v>
       </c>
@@ -3480,8 +3538,11 @@
       <c r="C29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E29" t="str">
+        <v>Aug</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A30" t="str">
         <v>Team Beta</v>
       </c>
@@ -3491,8 +3552,11 @@
       <c r="C30">
         <v>39</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E30" t="str">
+        <v>Sep</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A31" t="str">
         <v>Team Beta</v>
       </c>
@@ -3502,8 +3566,11 @@
       <c r="C31">
         <v>20</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E31" t="str">
+        <v>Oct</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A32" t="str">
         <v>Team Beta</v>
       </c>
@@ -3513,8 +3580,11 @@
       <c r="C32">
         <v>37</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E32" t="str">
+        <v>Nov</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A33" t="str">
         <v>Team Beta</v>
       </c>
@@ -3524,8 +3594,11 @@
       <c r="C33">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E33" t="str">
+        <v>Dec</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A34" t="str">
         <v>Team Gamma</v>
       </c>
@@ -3535,8 +3608,11 @@
       <c r="C34">
         <v>36</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E34" t="str">
+        <v>Jan</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A35" t="str">
         <v>Team Gamma</v>
       </c>
@@ -3546,8 +3622,11 @@
       <c r="C35">
         <v>39</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E35" t="str">
+        <v>Feb</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A36" t="str">
         <v>Team Gamma</v>
       </c>
@@ -3557,8 +3636,11 @@
       <c r="C36">
         <v>25</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E36" t="str">
+        <v>Mar</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A37" t="str">
         <v>Team Gamma</v>
       </c>
@@ -3568,8 +3650,11 @@
       <c r="C37">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E37" t="str">
+        <v>Apr</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A38" t="str">
         <v>Team Gamma</v>
       </c>
@@ -3579,8 +3664,11 @@
       <c r="C38">
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E38" t="str">
+        <v>May</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A39" t="str">
         <v>Team Gamma</v>
       </c>
@@ -3590,8 +3678,11 @@
       <c r="C39">
         <v>32</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E39" t="str">
+        <v>Jun</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A40" t="str">
         <v>Team Gamma</v>
       </c>
@@ -3601,8 +3692,11 @@
       <c r="C40">
         <v>28</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E40" t="str">
+        <v>Jul</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A41" t="str">
         <v>Team Gamma</v>
       </c>
@@ -3612,8 +3706,11 @@
       <c r="C41">
         <v>27</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E41" t="str">
+        <v>Aug</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A42" t="str">
         <v>Team Gamma</v>
       </c>
@@ -3623,8 +3720,11 @@
       <c r="C42">
         <v>21</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E42" t="str">
+        <v>Sep</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A43" t="str">
         <v>Team Gamma</v>
       </c>
@@ -3634,8 +3734,11 @@
       <c r="C43">
         <v>29</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E43" t="str">
+        <v>Oct</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A44" t="str">
         <v>Team Gamma</v>
       </c>
@@ -3645,8 +3748,11 @@
       <c r="C44">
         <v>21</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E44" t="str">
+        <v>Nov</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A45" t="str">
         <v>Team Gamma</v>
       </c>
@@ -3656,8 +3762,11 @@
       <c r="C45">
         <v>38</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E45" t="str">
+        <v>Dec</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A46" t="str">
         <v>Team Delta</v>
       </c>
@@ -3667,8 +3776,11 @@
       <c r="C46">
         <v>14</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E46" t="str">
+        <v>Jan</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A47" t="str">
         <v>Team Delta</v>
       </c>
@@ -3678,8 +3790,11 @@
       <c r="C47">
         <v>39</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E47" t="str">
+        <v>Feb</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A48" t="str">
         <v>Team Delta</v>
       </c>
@@ -3689,8 +3804,11 @@
       <c r="C48">
         <v>17</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E48" t="str">
+        <v>Mar</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A49" t="str">
         <v>Team Delta</v>
       </c>
@@ -3700,8 +3818,11 @@
       <c r="C49">
         <v>15</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E49" t="str">
+        <v>Apr</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A50" t="str">
         <v>Team Delta</v>
       </c>
@@ -3711,8 +3832,11 @@
       <c r="C50">
         <v>22</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E50" t="str">
+        <v>May</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A51" t="str">
         <v>Team Delta</v>
       </c>
@@ -3722,8 +3846,11 @@
       <c r="C51">
         <v>40</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E51" t="str">
+        <v>Jun</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A52" t="str">
         <v>Team Delta</v>
       </c>
@@ -3733,8 +3860,11 @@
       <c r="C52">
         <v>35</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E52" t="str">
+        <v>Jul</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A53" t="str">
         <v>Team Delta</v>
       </c>
@@ -3744,8 +3874,11 @@
       <c r="C53">
         <v>35</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E53" t="str">
+        <v>Aug</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A54" t="str">
         <v>Team Delta</v>
       </c>
@@ -3755,8 +3888,11 @@
       <c r="C54">
         <v>23</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E54" t="str">
+        <v>Sep</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A55" t="str">
         <v>Team Delta</v>
       </c>
@@ -3766,8 +3902,11 @@
       <c r="C55">
         <v>26</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E55" t="str">
+        <v>Oct</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A56" t="str">
         <v>Team Delta</v>
       </c>
@@ -3777,8 +3916,11 @@
       <c r="C56">
         <v>21</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E56" t="str">
+        <v>Nov</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A57" t="str">
         <v>Team Delta</v>
       </c>
@@ -3787,6 +3929,9 @@
       </c>
       <c r="C57">
         <v>25</v>
+      </c>
+      <c r="E57" t="str">
+        <v>Dec</v>
       </c>
     </row>
   </sheetData>
@@ -5949,7 +6094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E75372-233B-46C3-B60F-2EB456B82444}">
   <dimension ref="B2:N166"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>

</xml_diff>